<commit_message>
Uploaded file and fixed R code so Sanjana can add to MCH database
</commit_message>
<xml_diff>
--- a/NCES Data/FIPS_Codes.xlsx
+++ b/NCES Data/FIPS_Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcamp27\OneDrive - Emory University\Documents\GitHub\school_policy_mob\NCES Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC8282D-7B5C-4EDF-8AD1-37905739D06A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEB399F-FD33-4350-8C7F-579F4636DE95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4212" xr2:uid="{D3DDF903-6404-4CA3-9EBB-627ECDC08881}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6287" uniqueCount="1901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6287" uniqueCount="1902">
   <si>
     <t>FIPS</t>
   </si>
@@ -5728,6 +5728,9 @@
   </si>
   <si>
     <t>DeSoto</t>
+  </si>
+  <si>
+    <t>LaSalle</t>
   </si>
 </sst>
 </file>
@@ -6106,8 +6109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6082240A-BDCE-4E0C-A6C1-7084189FBB57}">
   <dimension ref="A1:C3143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A726" workbookViewId="0">
-      <selection activeCell="D747" sqref="D747"/>
+    <sheetView tabSelected="1" topLeftCell="A1521" workbookViewId="0">
+      <selection activeCell="B1544" sqref="B1544"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23093,7 +23096,7 @@
         <v>22059</v>
       </c>
       <c r="B1544" s="2" t="s">
-        <v>519</v>
+        <v>1901</v>
       </c>
       <c r="C1544" s="2" t="s">
         <v>759</v>

</xml_diff>